<commit_message>
Timesheet updated by Kirubaharan
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CADFEA2F-9AD3-4F38-8266-40345ED8C058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B2D4F63-140C-4FF9-97F9-64A673E4EDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
   <si>
     <t>Resource Name</t>
   </si>
@@ -201,6 +201,12 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>UI designing on trainer - landing page,feedback page</t>
+  </si>
+  <si>
+    <t>Trainer prototype completed,session about abstract pattern,Prototype disscussion with rafi,team discussion about modification on prototype</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prototype discussion with team </t>
   </si>
   <si>
@@ -210,6 +216,18 @@
     <t>Prototype design</t>
   </si>
   <si>
+    <t xml:space="preserve"> Discussion with team members about UI prototype - 40 mins, Worked on Acceptance criteria ,assumption and constraints for Trainee - 2 hours,Meeting with Rafi - 1 hour,  </t>
+  </si>
+  <si>
+    <t>Design pattern session - 40 mins ,softskill session- 50 mins,Others - 1 hour 20 mins</t>
+  </si>
+  <si>
+    <t>Trainer - constraints, acceptance criteria, assumptions</t>
+  </si>
+  <si>
+    <t>Wor,session about abstract pattern,Prototype disscussion with rafi,team discussion about modification on prototype</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arul </t>
   </si>
   <si>
@@ -219,7 +237,7 @@
     <t>Meeting with client - 45mins,I've discussed about UI protyping with team members - 45mins, Done acceptance criteria for Trainee user stories - 120 mins</t>
   </si>
   <si>
-    <t>Softskill Session-45 mins,others 90mins</t>
+    <t>Softskill Session-45 mins, Design pattern session ,others 90mins</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB7CC24-ECCE-4106-96A6-9EE0F697F084}">
   <dimension ref="B4:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1353,15 +1371,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43F9D7A-B406-44E1-9B23-838F510A10D3}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:8" ht="45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="81">
+    <row r="2" spans="1:8" ht="81">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1403,7 +1421,7 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="63.75">
+    <row r="3" spans="1:8" ht="63.75">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1424,7 +1442,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="78" customHeight="1">
+    <row r="4" spans="1:8" ht="78" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1441,28 +1459,26 @@
       </c>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:7" ht="71.25" customHeight="1">
+    <row r="5" spans="1:8" ht="71.25" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="B5" s="14"/>
       <c r="C5" s="5" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="13">
-        <v>0.22916666666666666</v>
-      </c>
       <c r="F5" s="13">
         <v>0.10416666666666667</v>
       </c>
       <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" ht="63.75">
+      <c r="H5" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="63.75">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1483,28 +1499,28 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="30.75">
+    <row r="7" spans="1:8" ht="81">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0.10416666666666667</v>
+        <v>59</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="63.75">
+    <row r="8" spans="1:8" ht="63.75">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1525,7 +1541,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="63.75">
+    <row r="9" spans="1:8" ht="63.75">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1546,7 +1562,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="102">
+    <row r="10" spans="1:8" ht="53.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1554,20 +1570,17 @@
         <v>18</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0.22916666666666666</v>
+        <v>62</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="F10" s="13">
         <v>0.10416666666666667</v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="83.25" customHeight="1">
+    <row r="11" spans="1:8" ht="83.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -1588,24 +1601,24 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="105.75" customHeight="1">
+    <row r="12" spans="1:8" ht="105.75" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G12" s="4"/>
     </row>

</xml_diff>

<commit_message>
Time Sheet updated by Sruthi
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B2D4F63-140C-4FF9-97F9-64A673E4EDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E17DFB1-7C92-4DB1-B7FD-7CA8AAB68DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="73">
   <si>
     <t>Resource Name</t>
   </si>
@@ -195,16 +195,22 @@
     <t>Session With Rafi(Builder Pattern)-30mins,Softskill Session-45 mins,others 20mins,Abstract Design Pattern-40mins ,Non Project-2:15 hrs</t>
   </si>
   <si>
-    <t>Design Pattern Session, Meeting with Client Rafi, Team Disscussion about Prototype, Making changes in Acceptance Cretiria, Constraints, Assumptions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>Design Pattern Session, Meeting with Client Rafi, , Making changes in Acceptance Cretiria, Constraints, Assumptions. Training Head - Acceptance Cretiria, Constraints, Assumptions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design Pattern Session-1 hr, Meeting with Client Rafi-45min, , Making changes in Acceptance Cretiria, Constraints, Assumptions. </t>
   </si>
   <si>
     <t>UI designing on trainer - landing page,feedback page</t>
   </si>
   <si>
-    <t>Trainer prototype completed,session about abstract pattern,Prototype disscussion with rafi,team discussion about modification on prototype</t>
+    <t>Previous UI design has been discarded</t>
+  </si>
+  <si>
+    <t>Worked on acceptance criteria and UI design - 1:30 mins,Prototype disscussion with rafi - 45 mins,team discussion about modification on prototype - 50 mins, Trainer Landpage,feedback page-1 hr</t>
+  </si>
+  <si>
+    <t>Abstract Pattern-40 mins,Softskill Session-45 mins,</t>
   </si>
   <si>
     <t xml:space="preserve">Prototype discussion with team </t>
@@ -222,10 +228,19 @@
     <t>Design pattern session - 40 mins ,softskill session- 50 mins,Others - 1 hour 20 mins</t>
   </si>
   <si>
+    <t>Meeting with rafi (reviewed UI design )-1hr</t>
+  </si>
+  <si>
     <t>Trainer - constraints, acceptance criteria, assumptions</t>
   </si>
   <si>
-    <t>Wor,session about abstract pattern,Prototype disscussion with rafi,team discussion about modification on prototype</t>
+    <t>Previous trainer UI design has been discarded</t>
+  </si>
+  <si>
+    <t>Worked on acceptance criteria and UI design - 1:30 mins,Prototype disscussion with rafi - 45 mins,team discussion about modification on prototype - 50 mins, Trainer - constraints, acceptance criteria, assumptions - 1 hr</t>
+  </si>
+  <si>
+    <t>Session with Rafi about abstract pattern - 40 mins</t>
   </si>
   <si>
     <t xml:space="preserve">Arul </t>
@@ -244,7 +259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +335,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -356,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -407,6 +434,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1065,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB7CC24-ECCE-4106-96A6-9EE0F697F084}">
   <dimension ref="B4:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1373,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43F9D7A-B406-44E1-9B23-838F510A10D3}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15"/>
@@ -1451,13 +1480,14 @@
         <v>53</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="14" t="s">
         <v>54</v>
       </c>
       <c r="F4" s="12">
         <v>0.10416666666666667</v>
       </c>
       <c r="G4" s="12"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="71.25" customHeight="1">
       <c r="A5" s="2" t="s">
@@ -1468,17 +1498,18 @@
         <v>55</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0.10416666666666667</v>
+        <v>56</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="63.75">
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="25.5">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1491,9 +1522,7 @@
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="13">
-        <v>0.22916666666666666</v>
-      </c>
+      <c r="E6" s="13"/>
       <c r="F6" s="13">
         <v>0.10416666666666667</v>
       </c>
@@ -1504,23 +1533,23 @@
         <v>20</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="63.75">
+    <row r="8" spans="1:8" ht="25.5">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1528,14 +1557,12 @@
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="13">
-        <v>0.22916666666666666</v>
-      </c>
+      <c r="E8" s="13"/>
       <c r="F8" s="13">
         <v>0.10416666666666667</v>
       </c>
@@ -1562,21 +1589,22 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="53.25">
+    <row r="10" spans="1:8" ht="94.5">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="13">
-        <v>0.10416666666666667</v>
+        <v>67</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -1603,22 +1631,22 @@
     </row>
     <row r="12" spans="1:8" ht="105.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G12" s="4"/>
     </row>

</xml_diff>

<commit_message>
TimeSheet updated by iswarya
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E17DFB1-7C92-4DB1-B7FD-7CA8AAB68DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F683837-F6DB-49B6-B8C8-698C0795B4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="77">
   <si>
     <t>Resource Name</t>
   </si>
@@ -195,10 +195,13 @@
     <t>Session With Rafi(Builder Pattern)-30mins,Softskill Session-45 mins,others 20mins,Abstract Design Pattern-40mins ,Non Project-2:15 hrs</t>
   </si>
   <si>
-    <t>Design Pattern Session, Meeting with Client Rafi, , Making changes in Acceptance Cretiria, Constraints, Assumptions. Training Head - Acceptance Cretiria, Constraints, Assumptions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design Pattern Session-1 hr, Meeting with Client Rafi-45min, , Making changes in Acceptance Cretiria, Constraints, Assumptions. </t>
+    <t>Training Head - Acceptance Cretiria, Constraints, Assumptions.</t>
+  </si>
+  <si>
+    <t>Meeting with Client Rafi-45min,Team Discussin about Prototype-50min , Making changes in Training Haed Acceptance Cretiria, Constraints, Assumptions-1hr.</t>
+  </si>
+  <si>
+    <t>Abstract Pattern Session-40min</t>
   </si>
   <si>
     <t>UI designing on trainer - landing page,feedback page</t>
@@ -229,6 +232,21 @@
   </si>
   <si>
     <t>Meeting with rafi (reviewed UI design )-1hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Meeting with rafi (reviewed UI design )-45mins
+Discussion with team about UI design-1hr
+Completed acceptance criteria,assumption,Contraints for training co-ordination 
+user stories.-2hrs
+Discussion with Kavin for UI design for training Co Ordinator-1hr
+</t>
+  </si>
+  <si>
+    <t>Landing page(Co ordinator)</t>
+  </si>
+  <si>
+    <t>Training head - UI designing ( Login page,dashboard,register page, View status page, Filter page)</t>
   </si>
   <si>
     <t>Trainer - constraints, acceptance criteria, assumptions</t>
@@ -1403,7 +1421,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15"/>
@@ -1471,7 +1489,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="78" customHeight="1">
+    <row r="4" spans="1:8" ht="103.5" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1483,8 +1501,8 @@
       <c r="E4" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="12">
-        <v>0.10416666666666667</v>
+      <c r="F4" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="18"/>
@@ -1495,16 +1513,16 @@
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="13"/>
@@ -1533,23 +1551,23 @@
         <v>20</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="25.5">
+    <row r="8" spans="1:8" ht="165.75">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1557,30 +1575,30 @@
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13">
-        <v>0.10416666666666667</v>
+      <c r="E8" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="63.75">
+    <row r="9" spans="1:8" ht="64.5" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="13">
         <v>0.22916666666666666</v>
       </c>
@@ -1589,22 +1607,22 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="94.5">
+    <row r="10" spans="1:8" ht="89.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -1631,22 +1649,22 @@
     </row>
     <row r="12" spans="1:8" ht="105.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G12" s="4"/>
     </row>

</xml_diff>

<commit_message>
timesheet updated by sobhana M
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7199A51-5D4D-466F-85F4-66A3C40A9302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{66325126-2B94-4D4E-A31A-CDE2BB4EB91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
     <sheet name="6-4-22 " sheetId="42" r:id="rId2"/>
     <sheet name="7-4-22" sheetId="43" r:id="rId3"/>
+    <sheet name="8-4-22" sheetId="44" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="119">
   <si>
     <t>Resource Name</t>
   </si>
@@ -321,6 +322,93 @@
   </si>
   <si>
     <t>Softskill Session-45 mins, Design pattern session ,others 90mins</t>
+  </si>
+  <si>
+    <t>Training Co-Ordinator(UI's)</t>
+  </si>
+  <si>
+    <t>Training Head(Dashboard,Manage Co-ordinator,List Of Trainee,Status Of Trainee),Training Co-ordinator(Course List),Entity Model</t>
+  </si>
+  <si>
+    <t>Meeting With Rafi -50 mins,Team Discussion-30 mins,UI Consistency-2 hrs: InOffice Total Time -3:20Hrs                 After 7:30-Working On UI Pages -4 hrs,Data Model-1 hr</t>
+  </si>
+  <si>
+    <t>Preaparing For PPt-2hrs,Builder and prototype pattern Session-1hr,Others -1 hr,In BasketBall Court -1 hr ,Total Time-5hr</t>
+  </si>
+  <si>
+    <t>ABSENT</t>
+  </si>
+  <si>
+    <t>Designing prototype</t>
+  </si>
+  <si>
+    <t>Entities and Data Model Rough</t>
+  </si>
+  <si>
+    <t>Meeting with client (Rafi) - 50mins, Team Discussion about Design and Entity - 120mins, Correction in Design - 60mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Builder Pattern Session-60min,  Photo Shoot at  BasketBall court - 60 mins, others(lunch &amp; tea break)-90min                         </t>
+  </si>
+  <si>
+    <t>Trainer Constraints and assumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting with Rafi -50 mins,Corrections in Design - 60 mins,Team discussion about entity and design -180 mins </t>
+  </si>
+  <si>
+    <t>Builder pattern session-60 mins,Friday activities-60 mins, Others - 90 mins</t>
+  </si>
+  <si>
+    <t>UI design for training co ordinator and Training head refining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training head login,register,Dashboard and List of department </t>
+  </si>
+  <si>
+    <t>Meeting with client (Rafi) - 50mins, Team Discussion about Design-120 min, Training head Design - 60mins and Prepare for presentation in Adaptor pattern-60 mina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern Session-60min,  Photo Shoot at  Volleyball court - 60 mins, others(lunch &amp; tea break)-1.15hour                         </t>
+  </si>
+  <si>
+    <t>Trainee acceptance criteria, Constraints and assumption</t>
+  </si>
+  <si>
+    <t>UI design (dashboard )for training co ordinator,entity framework and requirements</t>
+  </si>
+  <si>
+    <t>UI for trainee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting with Rafi -1hr(reviewed UI Design)Corrections in Design - 1hr,Team discussion about entity and design -2hrs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Builder Design Pattern and prototype Session-1hr,  Photo Shoot at  basketball court - 1hr, others(lunch &amp; tea break)-1.30hr                        </t>
+  </si>
+  <si>
+    <t>UI design (dashboard )for training co- ordinator</t>
+  </si>
+  <si>
+    <t>UI for training coordinator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting with Rafi -1hr,Corrections in Design - 1hr,Team discussion about entity and design -3hrs </t>
+  </si>
+  <si>
+    <t>Builder Design Pattern and prototype Session-1hr,  Photo Shoot at  basketball court - 1hr, others(lunch &amp; tea break)-1.30hr ,review-45min</t>
+  </si>
+  <si>
+    <t>Entities and Data model</t>
+  </si>
+  <si>
+    <t>Exploration</t>
+  </si>
+  <si>
+    <t>Meeting with client - 45mins,I've discussed about User flow team members - 120mins, Done entity model rough - 60 mins</t>
+  </si>
+  <si>
+    <t>Softskill -45 mins, Design pattern session ,others 90mins</t>
   </si>
 </sst>
 </file>
@@ -424,7 +512,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -447,11 +535,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -504,6 +601,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1470,7 +1573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43F9D7A-B406-44E1-9B23-838F510A10D3}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1721,4 +1824,257 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7951E731-BC0F-4432-8EF7-5AB4C8202D9B}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="73.5" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="100.5" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="160.5" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" ht="170.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="165" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="85.5" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="102.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="191.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="123.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="164.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="87" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated 9-4-22 Time Sheet
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{987EF940-B159-4F7B-A8C5-40675EDEEFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6996DBA7-7AD9-4139-ABBB-7FB49A9167ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="6-4-22 " sheetId="42" r:id="rId2"/>
     <sheet name="7-4-22" sheetId="43" r:id="rId3"/>
     <sheet name="8-4-22" sheetId="44" r:id="rId4"/>
+    <sheet name="9-4-22" sheetId="45" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="143">
   <si>
     <t>Resource Name</t>
   </si>
@@ -333,28 +334,37 @@
     <t>Meeting With Rafi -50 mins,Team Discussion-30 mins,UI Consistency-2 hrs: InOffice Total Time -3:20Hrs                 After 7:30-Working On UI Pages -4 hrs,Data Model-1 hr</t>
   </si>
   <si>
-    <t>Preaparing For PPt-2hrs,Builder and prototype pattern Session-1hr,Others -1 hr,In VolleyBall Court -1 hr ,Total Time-5hr</t>
-  </si>
-  <si>
-    <t>Training Head UI refining</t>
+    <t>Preaparing For PPt-2hrs,Builder and prototype pattern Session-1hr,Others -1 hr,In BasketBall Court -1 hr ,Total Time-5hr</t>
+  </si>
+  <si>
+    <t>ABSENT</t>
+  </si>
+  <si>
+    <t>Designing prototype</t>
+  </si>
+  <si>
+    <t>Entities and Data Model Rough</t>
   </si>
   <si>
     <t>Meeting with client (Rafi) - 50mins, Team Discussion about Design and Entity - 120mins, Correction in Design - 60mins</t>
   </si>
   <si>
-    <t xml:space="preserve">Builder Pattern Session-60min,  Photo Shoot at  Volleyball court - 60 mins, others(lunch &amp; tea break)-90min                         </t>
-  </si>
-  <si>
-    <t>UI design for training co ordinator</t>
-  </si>
-  <si>
-    <t>Training head refining</t>
-  </si>
-  <si>
-    <t>Meeting with client (Rafi) - 50mins, Team Discussion about Design-60 min, Correction in Design - 60mins and Prepare for presentation in Adaptor pattern-60 min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Builder Pattern Session-60min,  Photo Shoot at  Volleyball court - 60 mins, others(lunch &amp; tea break)-1.15hour                         </t>
+    <t xml:space="preserve">Builder Pattern Session-60min,  Photo Shoot at  BasketBall court - 60 mins, others(lunch &amp; tea break)-90min                         </t>
+  </si>
+  <si>
+    <t>Trainer course,topic,assignment,list of trinee and their detail page UI Design</t>
+  </si>
+  <si>
+    <t>UI design for training co ordinator and Training head refining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training head login,register,Dashboard and List of department </t>
+  </si>
+  <si>
+    <t>Meeting with client (Rafi) - 50mins, Team Discussion about Design-120 min, Training head Design - 60mins and Prepare for presentation in Adaptor pattern-60 mina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern Session-60min,  Photo Shoot at  Volleyball court - 60 mins, others(lunch &amp; tea break)-1.15hour                         </t>
   </si>
   <si>
     <t>Trainee acceptance criteria, Constraints and assumption</t>
@@ -366,20 +376,119 @@
     <t>Builder pattern session-60 mins,Friday activities-60 mins, Others - 90 mins</t>
   </si>
   <si>
-    <t>Entity and relationship model</t>
+    <t>UI design (dashboard )for training co ordinator,entity framework and requirements</t>
+  </si>
+  <si>
+    <t>UI for trainee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting with Rafi -1hr(reviewed UI Design)Corrections in Design - 1hr,Team discussion about entity and design -2hrs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Builder Design Pattern and prototype Session-1hr,  Photo Shoot at  basketball court - 1hr, others(lunch &amp; tea break)-1.30hr                        </t>
+  </si>
+  <si>
+    <t>UI design (dashboard )for training co- ordinator</t>
+  </si>
+  <si>
+    <t>UI for training coordinator</t>
   </si>
   <si>
     <t xml:space="preserve">Meeting with Rafi -1hr,Corrections in Design - 1hr,Team discussion about entity and design -3hrs </t>
   </si>
   <si>
-    <t xml:space="preserve">Builder Design Pattern and prototype Session-60min,  Photo Shoot at  basketball court - 60 mins, others(lunch &amp; tea break)-90min                         </t>
+    <t>Builder Design Pattern and prototype Session-1hr,  Photo Shoot at  basketball court - 1hr, others(lunch &amp; tea break)-1.30hr ,review-45min</t>
+  </si>
+  <si>
+    <t>Entities and Data model</t>
+  </si>
+  <si>
+    <t>Exploration</t>
+  </si>
+  <si>
+    <t>Meeting with client - 45mins,I've discussed about User flow team members - 120mins, Done entity model rough - 60 mins</t>
+  </si>
+  <si>
+    <t>Softskill -45 mins, Design pattern session ,others 90mins</t>
+  </si>
+  <si>
+    <t>Entity ,Attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training Co-ordinator(Review,Assignment),Consistent check in Training Co-ordinator </t>
+  </si>
+  <si>
+    <t>Team discussion - UI Integration -45 mins, Refining Flow Correction 2 hrs,Consistent Check-2hrs,ui design(Co-ordinator,Trainee) 2 hrs,Meeting With Rafi-1:45 hrs.Total 8:45 hrs</t>
+  </si>
+  <si>
+    <t>Break-1:00 hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Training head and training co-ordinator refining</t>
+  </si>
+  <si>
+    <t>Training Head UI page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>Team meeting -60mins ,Correction in  UI design-2hrs, entity frame work and datamodel -90 min ,Meeting with Rafi -1.45hours(reviewed UI Design)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">others(lunch &amp; tea break)-90min                         </t>
+  </si>
+  <si>
+    <t>Data Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training co-ordinator UI Discussion-1.30 hrs and design-3hrs,Meeting with Rafi -1.30 hrs. Sunday Trainer UI correction and Design-3hrs </t>
+  </si>
+  <si>
+    <t>UI design for training co ordinator (Assign course,review ,and attendance)</t>
+  </si>
+  <si>
+    <t>Ui design Training Co-ordinator Dashboard  and create course ,assign courseand prepare for presentation in design pattern</t>
+  </si>
+  <si>
+    <t>Prepare for presentation in design pattern -90 min ,Meeting with client (Rafi) - 1.45hours,Team meeting -60mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others(lunch &amp; tea break)-1.30hour                         </t>
+  </si>
+  <si>
+    <t>Consistency checking in Trainee, Entity modeling</t>
+  </si>
+  <si>
+    <t>Team discussion about UI integration - 45 mins , Entity modelling - 1 hour,consistency checking - 2 hours,review with Rafi - 100 mins</t>
+  </si>
+  <si>
+    <t>Lunch and other breaks - 1 hour 30 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI design for training co ordintor(schedule review),dashboard for training co-cordinator,trainee,trainer,training head, Entity framework and data model </t>
+  </si>
+  <si>
+    <t xml:space="preserve">others(lunch &amp; tea break)-1.30hr                        </t>
+  </si>
+  <si>
+    <t>Group discussion about UI integration - 45 mins , Entity modelling - 1 hour,Consistency checking - 2 hours,Session with Rafi - 100 mins</t>
+  </si>
+  <si>
+    <t>Lunch : 1hour, Break:20 mins</t>
+  </si>
+  <si>
+    <t>Break-2:00 hr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,6 +576,24 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -476,7 +603,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -499,11 +626,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,6 +692,21 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="B4:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:H20"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1522,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43F9D7A-B406-44E1-9B23-838F510A10D3}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15"/>
@@ -1779,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7951E731-BC0F-4432-8EF7-5AB4C8202D9B}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
@@ -1831,18 +1982,18 @@
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>54</v>
+      <c r="B3" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="12" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -1851,17 +2002,17 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="18"/>
@@ -1872,17 +2023,13 @@
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>63</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="13"/>
       <c r="G5" s="8"/>
       <c r="H5" s="13"/>
     </row>
@@ -1891,17 +2038,17 @@
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -1911,31 +2058,33 @@
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="12" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="213.75" customHeight="1">
+    <row r="8" spans="1:8" ht="102.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>108</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="13" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -1943,20 +2092,20 @@
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>76</v>
+      <c r="B9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>78</v>
+        <v>94</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -1964,18 +2113,17 @@
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>82</v>
+        <v>94</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -1984,19 +2132,19 @@
         <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>85</v>
+        <v>113</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -2005,19 +2153,270 @@
         <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>89</v>
+        <v>118</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A377B9-DC0C-451C-B12D-A0709E33CEF2}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="73.5" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:8" ht="100.5" customHeight="1">
+      <c r="A3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="160.5" customHeight="1">
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" ht="170.25" customHeight="1">
+      <c r="A5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="165" customHeight="1">
+      <c r="A6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="85.5" customHeight="1">
+      <c r="A7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="102.75" customHeight="1">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="191.25" customHeight="1">
+      <c r="A9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="123.75" customHeight="1">
+      <c r="A10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="164.25" customHeight="1">
+      <c r="A11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="87" customHeight="1">
+      <c r="A12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="G12" s="4"/>
     </row>

</xml_diff>

<commit_message>
Timesheet updated by Gokul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDED8853-5A91-4291-B6B6-DDF45B60851A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB3268C7-76E9-4537-AE35-1A520406CE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="165">
   <si>
     <t>Resource Name</t>
   </si>
@@ -497,6 +497,18 @@
     <t>Trainer UI</t>
   </si>
   <si>
+    <t>Entity relationships, Entity attributes</t>
+  </si>
+  <si>
+    <t>Completed Changes in Trainee Design, Completed changes in Trainer Design, Worked on Data Models in TMS</t>
+  </si>
+  <si>
+    <t>Changes in Trainee Design - 2hr,Meeting With Rafi - 1hr 30 mins, Data Models - 1hr 30 mins total hrs- 5hrs</t>
+  </si>
+  <si>
+    <t>Lunch and break 1hr 15 mins, self exploration - entity frame work - 1hr total hrs - 2 hrs 15 mins</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Data model Relationship </t>
   </si>
   <si>
@@ -509,10 +521,34 @@
     <t>Designing Entity data model for Trainee</t>
   </si>
   <si>
-    <t>Data model</t>
-  </si>
-  <si>
-    <t>Meeting with client - 90 mins, I've decided to work on entity data for  members - 120mins, Done entity model rough - 60 mins</t>
+    <t>Reviewed acceptance criteria for Trainee ,Trainer,training coordinator,Training head, Updated MOM</t>
+  </si>
+  <si>
+    <t>Discussion with team - 20 mins, Worked on entity data model for trainee and collaborated with others-120  mins,meeting with Rafi- 100 mins</t>
+  </si>
+  <si>
+    <t>Prepared for code review - 1 hour , others - 90 mins</t>
+  </si>
+  <si>
+    <t>Data model Relationship</t>
+  </si>
+  <si>
+    <t>Entities and attributes for entire flow</t>
+  </si>
+  <si>
+    <t>Team discussion-15 mins,working with Data model-2hrs, Meeting with client (Rafi) - 1.30 hrs,Prepared data model for entire flow - 3 hrs</t>
+  </si>
+  <si>
+    <t>Break - 1 hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed acceptance criteria for Trainee, Trainer, Training co ordinator, Trainnig Head. </t>
+  </si>
+  <si>
+    <t>Meeting with client - 90 mins, I've decided to work on entity data model for trainee and Integrated others- 120mins, Done entity model rough - 60 mins</t>
+  </si>
+  <si>
+    <t>lunch and others 130mins</t>
   </si>
 </sst>
 </file>
@@ -652,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -710,6 +746,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,7 +1090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="B4:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2182,7 +2221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A377B9-DC0C-451C-B12D-A0709E33CEF2}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
   <sheetData>
@@ -2429,8 +2468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996EE506-C210-4575-ABFA-32B522DBF415}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
@@ -2485,17 +2524,17 @@
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>94</v>
+        <v>147</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>148</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="12" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>94</v>
+        <v>150</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -2524,17 +2563,17 @@
         <v>17</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="14" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="13"/>
@@ -2563,17 +2602,17 @@
         <v>20</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>104</v>
+        <v>155</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="12" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -2622,19 +2661,17 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>94</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="D10" s="14"/>
       <c r="E10" s="14" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -2664,17 +2701,19 @@
         <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="5"/>
+        <v>154</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="D12" s="5" t="s">
         <v>116</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>118</v>
+        <v>164</v>
       </c>
       <c r="G12" s="4"/>
     </row>

</xml_diff>

<commit_message>
Timesheet updated by Asuvath
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4633F83A-EFEC-402F-B148-C9E2D5C1F140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25287550-B431-47C2-AEF2-271F41ACA22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="211">
   <si>
     <t>Resource Name</t>
   </si>
@@ -606,6 +606,18 @@
     <t>lunch and others 130mins</t>
   </si>
   <si>
+    <t>Data model (Behaviours)</t>
+  </si>
+  <si>
+    <t>UI(Trainer)</t>
+  </si>
+  <si>
+    <t>Team,Discussion 30mins,iUI(Trainer)-2hrs,Meeting With Rafi-1 hr-total -3:30 hrs</t>
+  </si>
+  <si>
+    <t>session with anitha(1hr),Preaparation for Presentation-3hrs,Total-4 hrs</t>
+  </si>
+  <si>
     <t xml:space="preserve">team meeting - 30 mins,TMS data model refining - 2 hr 30 mins, Data entry in TMS - 30 mins, TMS relation ship mapping - 30 mins, rafi meeting - 1hr, MOM - 30 mins </t>
   </si>
   <si>
@@ -618,7 +630,10 @@
     <t>Date model, relationships and behaviour</t>
   </si>
   <si>
-    <t>TMS Full UI Prototype</t>
+    <t>TMS Full UI Design Flow</t>
+  </si>
+  <si>
+    <t>Team Disscussion 30 mins about Design Integration and Data Model, Integration on Training Head, Co-ordinator, Trainer, Trainee design flow 100 mins, Meeting with client (Rafi) - 60mins, Creating Reviewer Flow and Making Changes in Course Flow 60mins, Finalize the TMS Design Flow 120mins</t>
   </si>
   <si>
     <t>Class model with operations</t>
@@ -642,6 +657,9 @@
     <t xml:space="preserve">Meeting with Rafi-60 minutes,Worked on Trainer, and Trainee  naming conversion and consistency-2 hours ,Discussion with team - 30mins </t>
   </si>
   <si>
+    <t xml:space="preserve">others(lunch &amp; tea break)-100 min                       </t>
+  </si>
+  <si>
     <t>Behaviours of entity and view  models</t>
   </si>
   <si>
@@ -657,7 +675,7 @@
     <t>Team meeting - 30 mins, Refining Entities and attributes for TMS - 2 hr 30 mins,  rafi meeting - 1hr,  Relationship mapping -  30 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">Full Ui design completed </t>
+    <t xml:space="preserve">Full UI design completed </t>
   </si>
   <si>
     <t>Relationship mapping</t>
@@ -2849,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72FD7D6-2E49-4D32-923A-F7B61A1B2E55}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
@@ -2887,17 +2905,17 @@
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="12" t="s">
-        <v>92</v>
+        <v>185</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -2907,14 +2925,14 @@
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="22" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="12" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -2923,14 +2941,14 @@
         <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="14" t="s">
-        <v>153</v>
+        <v>192</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>154</v>
@@ -2943,17 +2961,17 @@
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="24" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="13"/>
@@ -2963,17 +2981,17 @@
         <v>19</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="14" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -2982,17 +3000,17 @@
         <v>20</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="13" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -3004,11 +3022,11 @@
         <v>165</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="22" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>160</v>
@@ -3023,7 +3041,7 @@
         <v>168</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
@@ -3039,17 +3057,17 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="22" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -3065,7 +3083,7 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="22" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
Timesheet updated by Arul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25287550-B431-47C2-AEF2-271F41ACA22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{539BF08A-6DDE-437E-A6CA-D705D000C912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="214">
   <si>
     <t>Resource Name</t>
   </si>
@@ -648,7 +648,7 @@
     <t>Session with Anitha-1 hr, worked with assignments given by anitha, Break - 1:30 hrs</t>
   </si>
   <si>
-    <t>Entity data model,Flow of UI design</t>
+    <t>Entity Date Model and Relationships</t>
   </si>
   <si>
     <t>UI design Consistency for Trainee and trainer</t>
@@ -678,6 +678,9 @@
     <t xml:space="preserve">Full UI design completed </t>
   </si>
   <si>
+    <t xml:space="preserve">discussion with team -30min,intergation of head ,co ordinator , trainer , trainee UI-100mins, meeting rafi 60 mins , creating reviewer work flow design and editing the course list - 60mis, reviewing the full uI work flow -120min. </t>
+  </si>
+  <si>
     <t>Relationship mapping</t>
   </si>
   <si>
@@ -688,6 +691,12 @@
   </si>
   <si>
     <t>Team discussion- 30 mins, Meeting with rafi - 1hr, MOM - 30 mins ,Entities and attributes for TMS - 2 hr 30 mins, Relationship mapping -  30 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data entry in TMS - 30 mins, TMS relation ship mapping - 30 mins, rafi meeting - 1hr, MOM - 30 mins </t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins, client meeting - 1hr, Refining Entities and attributes for TMS - 2 hr 30 mins,MOM - 30 mins , Relationship mapping -  30 mins</t>
   </si>
 </sst>
 </file>
@@ -2868,7 +2877,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
@@ -3045,7 +3054,7 @@
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>171</v>
@@ -3060,14 +3069,14 @@
         <v>193</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -3083,7 +3092,7 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>179</v>
@@ -3095,16 +3104,16 @@
         <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>116</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Timesheet updated by Sobhana
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{539BF08A-6DDE-437E-A6CA-D705D000C912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83FCB9BF-B47F-45F7-BC32-B28A4DE47E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2876,8 +2876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72FD7D6-2E49-4D32-923A-F7B61A1B2E55}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Timesheet update by Arul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25217"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83FCB9BF-B47F-45F7-BC32-B28A4DE47E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3125AA60-0704-4174-9861-4EA9B7AEDDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
@@ -20,8 +20,12 @@
     <sheet name="9-4-22" sheetId="45" r:id="rId5"/>
     <sheet name="11-4-22" sheetId="46" r:id="rId6"/>
     <sheet name="12-4-22" sheetId="47" r:id="rId7"/>
+    <sheet name="13-4-22 " sheetId="48" r:id="rId8"/>
+    <sheet name="15-4-22  " sheetId="49" r:id="rId9"/>
+    <sheet name="18-04-22" sheetId="51" r:id="rId10"/>
+    <sheet name="19-04-22 " sheetId="52" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="311">
   <si>
     <t>Resource Name</t>
   </si>
@@ -624,7 +650,7 @@
     <t>4hrs 30 mins</t>
   </si>
   <si>
-    <t>Lunch &amp; break - 1hr 30 mins,</t>
+    <t>Lunch &amp; break - 1hr 30 mins,teaching others - 1hr</t>
   </si>
   <si>
     <t>Date model, relationships and behaviour</t>
@@ -697,13 +723,308 @@
   </si>
   <si>
     <t>Team meeting - 30 mins, client meeting - 1hr, Refining Entities and attributes for TMS - 2 hr 30 mins,MOM - 30 mins , Relationship mapping -  30 mins</t>
+  </si>
+  <si>
+    <t>Trainer (ui)</t>
+  </si>
+  <si>
+    <t>Correcting work flow of trainee and reviewing the co-ordinator.</t>
+  </si>
+  <si>
+    <t>team discussion 30 mins,working on ui(trainee)-1 hr and 30 mins ,meeting with rafi 30 mins,working refining data model -1 hr,working on ui reviewing and consistent check(over all)-2:30hrs ,Total-5hrs and 30 mins</t>
+  </si>
+  <si>
+    <t>break 1 hr</t>
+  </si>
+  <si>
+    <t>TMS Physical Data Model,TMS calss diagram with operations</t>
+  </si>
+  <si>
+    <t>team meeting - 30 mins,TMS data model refining - 2 hr 30 mins, Data entry in TMS - 30 mins, TMS relation ship mapping - 30 mins, rafi meeting - 1hr</t>
+  </si>
+  <si>
+    <t>Review the Entire UI and relationship of datamodel</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins, Relationship for Datamodel -30 mis, Understanding the 2 different datamodel-1 hr ,Team discussion for Datamodel relationship-2hr, Review the entire UI -2hr</t>
+  </si>
+  <si>
+    <t>Lunch and tea break -1.30 mins</t>
+  </si>
+  <si>
+    <t>UI for Trainer in TMS</t>
+  </si>
+  <si>
+    <t>UI design work flowfor Training Co-ordinator and Trainer</t>
+  </si>
+  <si>
+    <t>Team meeting - 1.30hr, rafi meeting - 30mins,Entity data model relationship and UI design Trainee -2hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">others(lunch &amp; tea break)-90min                       </t>
+  </si>
+  <si>
+    <t>Entity data model operation for TMS</t>
+  </si>
+  <si>
+    <t>Entity datamodel ,artributes for TMS</t>
+  </si>
+  <si>
+    <t>Team meeting - 1.30hr, rafi meeting - 30mins,Entity data model relationship ,attributes,operation-2hrs</t>
+  </si>
+  <si>
+    <t>Review the Entire UI</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins, Understanding the datamodel-1 hr ,Team discussion for Datamodel relationship-2hr, Review the entire UI -2hr</t>
+  </si>
+  <si>
+    <t>Refining the data model</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins, Understanding the datamodel-1 hr ,Team discussion for Datamodel relationship-2hr,Refining the data model -30 min</t>
+  </si>
+  <si>
+    <t>view model for a page</t>
+  </si>
+  <si>
+    <t>TMS physical model</t>
+  </si>
+  <si>
+    <t>Team discussion- 30 mins, Meeting with rafi - 1hr, MOM - 30 mins , Relationship mapping -  30 mins</t>
+  </si>
+  <si>
+    <t>HLD</t>
+  </si>
+  <si>
+    <t>UI(Trainer),Overall(consistent check),reviewing data model.</t>
+  </si>
+  <si>
+    <t>Team meet -20 mins,working on ui(over all)-3hrs,reviewing data model and convey the corrections-30mins,reviewing trainer(constraints,assumption,acceptance criteria)-30mins,</t>
+  </si>
+  <si>
+    <t>break -1:30 hrs</t>
+  </si>
+  <si>
+    <t>angular cli exploration</t>
+  </si>
+  <si>
+    <t>TMS Physical Data Model - 1 hr, TMS class diagram - 1 hr, TMS class diagram with operations - 1hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> angular cli cmd - 1hr 30 mins,lunch and break- 1hr                          </t>
+  </si>
+  <si>
+    <t>checking overall UI flow and checking flow , acceptance criteria, assumption, constraints</t>
+  </si>
+  <si>
+    <t>team meet 20mins, checking and editing overall UI -3hrs,  checking flow , acceptance criteria, assumption, constraints (training head)- 30mis</t>
+  </si>
+  <si>
+    <t>Refining the Trainer and Head Acceptance Criteria,constrain,assumption</t>
+  </si>
+  <si>
+    <t>Team meet in online-20 mins, Review the physical datamodel and class diagram-1hr, trainer and head Acceptance criteria,constrain and assumption-2hrs, review the trainig coordinator Acceptance criteria-20 mins</t>
+  </si>
+  <si>
+    <t>UI(Trainer),Overall(consistent check) in UI prototype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Refined acceptance criteria for trainee flow</t>
+  </si>
+  <si>
+    <t>Team meet - 20 mins , Reviewed acceptance criteria for trainee - 2 hours , TMS physical data model - 1 hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunch - 1 hour </t>
+  </si>
+  <si>
+    <t>Refining the Training coordinator Acceptance Criteria,constrain,assumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team meet in online-20 mins, Review the physical datamodel and class diagram-1hr, training coordinator Acceptance criteria,constrain and assumption-2hrs, </t>
+  </si>
+  <si>
+    <t>lunch -1hr</t>
+  </si>
+  <si>
+    <t>Refining the Trainer and Head Acceptance Criteria,constrain</t>
+  </si>
+  <si>
+    <t>View model for a page</t>
+  </si>
+  <si>
+    <t>Physical Data model and acceptance criteria and assumption and constrains for trainee</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Entity Framework(self exploration)</t>
+  </si>
+  <si>
+    <t>meeting with team-30 mins(HLD)</t>
+  </si>
+  <si>
+    <t>Preparing for review(webapi)-3 hrs,self exploration-2 hrs.total-5 hrs</t>
+  </si>
+  <si>
+    <t>Explored Angular components, data binding, passing data from parent to child, from child to parent, life cycles of angular components etc.</t>
+  </si>
+  <si>
+    <t>Team discussion 30mins</t>
+  </si>
+  <si>
+    <t>angular 5hrs, typescript 30mins, lunch and break 1hr 30mins</t>
+  </si>
+  <si>
+    <t>HLD for TMS</t>
+  </si>
+  <si>
+    <t>Self Exploration</t>
+  </si>
+  <si>
+    <t>Team discussion -30mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lunch and Tea break-90min,Basics and overview of Entity framework,web api,angular.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 mins : Team discussion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1hr : WebAPI basic 2hrs : Angular 1hr : implemented the learned concept </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 mins : Team discussion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1hr : WebAPI basic 2hrs : c# 1hr : implemented the learned concept </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explored on Angular 1 hour30 mins , Web API basics 1 hour 30 mins </t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins</t>
+  </si>
+  <si>
+    <t>Others ( Lunch and  Tea break)-1 hour 30 mins</t>
+  </si>
+  <si>
+    <t>30 mins : Team discussion</t>
+  </si>
+  <si>
+    <t>exploration on entity framework, and web API-2.30hrs</t>
+  </si>
+  <si>
+    <t>self Exploration</t>
+  </si>
+  <si>
+    <t>lunch -1.30hr exploration on entity framework, and web API -2hrs</t>
+  </si>
+  <si>
+    <t>Team discussion about Hld - 30 mins</t>
+  </si>
+  <si>
+    <t>basic concepts on angular and web api- 3 hrs, lunch break - 1 hr</t>
+  </si>
+  <si>
+    <t>Lunch -45mins,Break-20 min,exploration on entity framework,  web API -1.30min,Install and run the typescript code-45mins,</t>
+  </si>
+  <si>
+    <t>Exploration on Angular, Entity Framework</t>
+  </si>
+  <si>
+    <t>angular exploration</t>
+  </si>
+  <si>
+    <t>system architecture</t>
+  </si>
+  <si>
+    <t>Team discussion 30mins, system architecture - 1 hr, reviewed data dictonary - 30mins,helped in view model - 30 mins,</t>
+  </si>
+  <si>
+    <t>angular 4hrs,  lunch and break 1hr 30mins</t>
+  </si>
+  <si>
+    <t>Layout for Login and Navbar</t>
+  </si>
+  <si>
+    <t>team meet 30mins, Html and Css Layout for Side navbar and Login page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review with Anitha - 60mins, Lunch and Tea break-90min,Typescript overview and basic program,  </t>
+  </si>
+  <si>
+    <t>View Model for TMS. Non-functional Requirements in HLD</t>
+  </si>
+  <si>
+    <t>30mins : Team discussion, 1hr : View model,1hr : non-functional Requirements,</t>
+  </si>
+  <si>
+    <t>3hr : Exploring Angular 1hr: Exploring Typescript</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Angular exploration</t>
+  </si>
+  <si>
+    <t>Flow chart for Trainee flow</t>
+  </si>
+  <si>
+    <t>Angular 1 hour 30 mins, re explored the concepts of SQL and C# - 2 hours,Worked on assignment Given by Jaya - 1 hour 30 mins Others ( Lunch and  Tea break)-1 hour 30 mins</t>
+  </si>
+  <si>
+    <t>exploration on web api</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins
+HLD for tms - 1 hr</t>
+  </si>
+  <si>
+    <t>Preparation for internal review - 30 min
+Internal review - 1 hr
+Lunch &amp; Tea break - 1.5 hr
+Typescript overview - 30 mins</t>
+  </si>
+  <si>
+    <t>team discussion - 30min, Html and css layout for sidesnavbar and login page.</t>
+  </si>
+  <si>
+    <t>lunch -1.30hr , exploring typescript.</t>
+  </si>
+  <si>
+    <t>View Model for TMS. Design Principles and introduction in HLD</t>
+  </si>
+  <si>
+    <t>Team discussion - 30 mins,View model - 1hr</t>
+  </si>
+  <si>
+    <t>Explored on angular - 2hrs,typescript - 1 hr</t>
+  </si>
+  <si>
+    <t>Data Model and Database discription of HLD</t>
+  </si>
+  <si>
+    <t>Team meeting-30 mins,Typescript-30mins,Database discription of HLD-2hrs, Exploration on Entity framework and Angular -45min</t>
+  </si>
+  <si>
+    <t>Typescript exploration</t>
+  </si>
+  <si>
+    <t>TMS logical view and Component identifing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team meeting - 30 mins, Logical view of TMS - 30 mins, </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,6 +1112,24 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -800,7 +1139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -832,11 +1171,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -903,6 +1277,42 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1558,6 +1968,520 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA24D0C2-D6B3-4372-947D-77C8110E9B72}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.5">
+      <c r="A2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="1:7" ht="51">
+      <c r="A3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="58.5" customHeight="1">
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="130.5" customHeight="1">
+      <c r="A5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7" ht="25.5">
+      <c r="A6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="25.5">
+      <c r="A7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="55.5" customHeight="1">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="25.5">
+      <c r="A9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="85.5" customHeight="1">
+      <c r="A10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="57.75" customHeight="1">
+      <c r="A11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="141" customHeight="1">
+      <c r="A12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95F4A8A-E29B-4E18-8E69-E97113C33CFB}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.5">
+      <c r="A2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="1:7" ht="40.5">
+      <c r="A3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="100.5" customHeight="1">
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="130.5" customHeight="1">
+      <c r="A5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="67.5">
+      <c r="A7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="82.5" customHeight="1">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="27">
+      <c r="A9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="85.5" customHeight="1">
+      <c r="A10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="110.25" customHeight="1">
+      <c r="A11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="141" customHeight="1">
+      <c r="A12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB7CC24-ECCE-4106-96A6-9EE0F697F084}">
   <dimension ref="B4:H20"/>
@@ -1876,7 +2800,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="45">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1899,7 +2823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="81">
+    <row r="2" spans="1:8" ht="61.5">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1918,7 +2842,7 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="53.25">
+    <row r="3" spans="1:8" ht="37.5">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1977,7 +2901,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:8" ht="148.5">
+    <row r="6" spans="1:8" ht="123">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1998,7 +2922,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="81">
+    <row r="7" spans="1:8" ht="74.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -2017,7 +2941,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="161.25">
+    <row r="8" spans="1:8" ht="147">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -2057,7 +2981,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="94.5">
+    <row r="10" spans="1:8" ht="86.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -2133,7 +3057,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="45">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2622,7 +3546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996EE506-C210-4575-ABFA-32B522DBF415}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16:C17"/>
     </sheetView>
   </sheetViews>
@@ -2631,7 +3555,7 @@
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2876,7 +3800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72FD7D6-2E49-4D32-923A-F7B61A1B2E55}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2886,7 +3810,7 @@
     <col min="3" max="3" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45">
+    <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3116,6 +4040,492 @@
         <v>213</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD081811-85A5-4B2D-B88E-0FFF35F2A58F}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="73.5" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="100.5" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="160.5" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" ht="170.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="165" customHeight="1">
+      <c r="A6" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="85.5" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="102.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="191.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="123.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="164.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="87" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8529FBE3-AC7C-4AEE-8C76-4DFCE0A834B0}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="27" t="e" cm="1">
+        <f t="array" aca="1" ref="A1" ca="1">--B</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="73.5" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="1:8" ht="100.5" customHeight="1">
+      <c r="A3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="160.5" customHeight="1">
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" ht="170.25" customHeight="1">
+      <c r="A5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" ht="165" customHeight="1">
+      <c r="A6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="85.5" customHeight="1">
+      <c r="A7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="102.75" customHeight="1">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="191.25" customHeight="1">
+      <c r="A9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="123.75" customHeight="1">
+      <c r="A10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="164.25" customHeight="1">
+      <c r="A11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="87" customHeight="1">
+      <c r="A12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>182</v>
       </c>
       <c r="G12" s="4"/>

</xml_diff>

<commit_message>
gokul updated time sheet
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{618D25B2-4A93-48B8-86FC-8040DA65A57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD13025A-B1AF-47B8-A2A7-EBE5D3BBB173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
@@ -24,8 +24,9 @@
     <sheet name="15-4-22  " sheetId="49" r:id="rId9"/>
     <sheet name="18-04-22" sheetId="51" r:id="rId10"/>
     <sheet name="19-04-22 " sheetId="52" r:id="rId11"/>
+    <sheet name="20-04-22" sheetId="53" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="320">
   <si>
     <t>Resource Name</t>
   </si>
@@ -779,6 +780,12 @@
     <t>Team meeting - 30 mins, Understanding the datamodel-1 hr ,Team discussion for Datamodel relationship-2hr, Review the entire UI -2hr</t>
   </si>
   <si>
+    <t>Refining the data model</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins, Understanding the datamodel-1 hr ,Team discussion for Datamodel relationship-2hr,Refining the data model -30 min</t>
+  </si>
+  <si>
     <t>view model for a page</t>
   </si>
   <si>
@@ -833,10 +840,10 @@
     <t xml:space="preserve">Lunch - 1 hour </t>
   </si>
   <si>
-    <t>Acceptance criteria ,assumption,dependencies ,user stories for training co ordinator</t>
-  </si>
-  <si>
-    <t>Team meeting - 30mins, Refining user stories,acceptance creteria ,dependencies,assumption for training co ordinator-2.30hrs</t>
+    <t>Refining the Training coordinator Acceptance Criteria,constrain,assumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team meet in online-20 mins, Review the physical datamodel and class diagram-1hr, training coordinator Acceptance criteria,constrain and assumption-2hrs, </t>
   </si>
   <si>
     <t>lunch -1hr</t>
@@ -878,12 +885,24 @@
     <t>Self Exploration</t>
   </si>
   <si>
+    <t>Team discussion -30mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lunch and Tea break-90min,Basics and overview of Entity framework,web api,angular.</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 mins : Team discussion </t>
   </si>
   <si>
     <t xml:space="preserve">1hr : WebAPI basic 2hrs : Angular 1hr : implemented the learned concept </t>
   </si>
   <si>
+    <t xml:space="preserve">31 mins : Team discussion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1hr : WebAPI basic 2hrs : c# 1hr : implemented the learned concept </t>
+  </si>
+  <si>
     <t xml:space="preserve">Explored on Angular 1 hour30 mins , Web API basics 1 hour 30 mins </t>
   </si>
   <si>
@@ -899,12 +918,21 @@
     <t>exploration on entity framework, and web API-2.30hrs</t>
   </si>
   <si>
+    <t>self Exploration</t>
+  </si>
+  <si>
+    <t>lunch -1.30hr exploration on entity framework, and web API -2hrs</t>
+  </si>
+  <si>
     <t>Team discussion about Hld - 30 mins</t>
   </si>
   <si>
     <t>basic concepts on angular and web api- 3 hrs, lunch break - 1 hr</t>
   </si>
   <si>
+    <t>Lunch -45mins,Break-20 min,exploration on entity framework,  web API -1.30min,Install and run the typescript code-45mins,</t>
+  </si>
+  <si>
     <t>Exploration on Angular, Entity Framework</t>
   </si>
   <si>
@@ -918,6 +946,106 @@
   </si>
   <si>
     <t>angular 4hrs,  lunch and break 1hr 30mins</t>
+  </si>
+  <si>
+    <t>Layout for Login and Navbar</t>
+  </si>
+  <si>
+    <t>team meet 30mins, Html and Css Layout for Side navbar and Login page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review with Anitha - 60mins, Lunch and Tea break-90min,Typescript overview and basic program,  </t>
+  </si>
+  <si>
+    <t>View Model for TMS. Non-functional Requirements in HLD</t>
+  </si>
+  <si>
+    <t>30mins : Team discussion, 1hr : View model,1hr : non-functional Requirements,</t>
+  </si>
+  <si>
+    <t>3hr : Exploring Angular 1hr: Exploring Typescript</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Angular exploration</t>
+  </si>
+  <si>
+    <t>Flow chart for Trainee flow</t>
+  </si>
+  <si>
+    <t>Angular 1 hour 30 mins, re explored the concepts of SQL and C# - 2 hours,Worked on assignment Given by Jaya - 1 hour 30 mins Others ( Lunch and  Tea break)-1 hour 30 mins</t>
+  </si>
+  <si>
+    <t>exploration on web api</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins
+HLD for tms - 1 hr</t>
+  </si>
+  <si>
+    <t>Preparation for internal review - 30 min
+Internal review - 1 hr
+Lunch &amp; Tea break - 1.5 hr
+Typescript overview - 30 mins</t>
+  </si>
+  <si>
+    <t>team discussion - 30min, Html and css layout for sidesnavbar and login page.</t>
+  </si>
+  <si>
+    <t>lunch -1.30hr , exploring typescript.</t>
+  </si>
+  <si>
+    <t>View Model for TMS. Design Principles and introduction in HLD</t>
+  </si>
+  <si>
+    <t>Team discussion - 30 mins,View model - 1hr</t>
+  </si>
+  <si>
+    <t>Explored on angular - 2hrs,typescript - 1 hr</t>
+  </si>
+  <si>
+    <t>Data Model and Database discription of HLD</t>
+  </si>
+  <si>
+    <t>Team meeting-30 mins,Typescript-30mins,Database discription of HLD-2hrs, Exploration on Entity framework and Angular -45min</t>
+  </si>
+  <si>
+    <t>Typescript exploration</t>
+  </si>
+  <si>
+    <t>TMS logical view and Component identifing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team meeting - 30 mins, Logical view of TMS - 30 mins, </t>
+  </si>
+  <si>
+    <t>web api exploration</t>
+  </si>
+  <si>
+    <t>team meeting - 30 mins, Meeting with rafi 1hr,  team discussion -1hr, web api - 2hr</t>
+  </si>
+  <si>
+    <t>4hrs 30mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lunch and break 1hr 30mins, clearing others doubts - 2hrs </t>
+  </si>
+  <si>
+    <t>Interactions in HLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30mins : Team discussion, 1hr : Meeting With Rafi, 35mins : Session about HLD and services, 30mins : Team discussion for splitting the topics and doubt clarification, 1 hr :System Architecture and NFA for HLD  </t>
+  </si>
+  <si>
+    <t>3omis : Component concept in Angular,1 hrs : Softskill session,1.30 mins : Break time</t>
+  </si>
+  <si>
+    <t>Team discussion for 30 mins, meeting with rafi for 35 mins,Session on Hld and services, Discussion with team for splitting topics and doubt clarification - 30 mins,Worked on system architecture and NFA for Hld,Data model - 30 mins</t>
+  </si>
+  <si>
+    <t>Softskill session - 1 he,  break - 1:30 mins</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1213,6 +1341,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1872,8 +2003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA24D0C2-D6B3-4372-947D-77C8110E9B72}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1889,7 +2020,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30">
       <c r="A1" s="27" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>4</v>
@@ -1915,17 +2046,17 @@
         <v>9</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G2" s="28"/>
     </row>
@@ -1934,36 +2065,36 @@
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="35" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="178.5">
+    <row r="4" spans="1:7" ht="58.5" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>190</v>
+        <v>265</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>243</v>
+        <v>267</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>154</v>
+        <v>268</v>
       </c>
       <c r="G4" s="13"/>
     </row>
@@ -1972,36 +2103,36 @@
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="24" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:7" ht="178.5">
+    <row r="6" spans="1:7" ht="25.5">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>235</v>
+      <c r="B6" s="23" t="s">
+        <v>265</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="D6" s="14"/>
-      <c r="E6" s="14" t="s">
-        <v>199</v>
+      <c r="E6" s="24" t="s">
+        <v>271</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>200</v>
+        <v>272</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -2010,17 +2141,17 @@
         <v>20</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -2029,36 +2160,36 @@
         <v>21</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="24" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="178.5">
+    <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>168</v>
+        <v>265</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -2067,36 +2198,36 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="34" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="51">
+    <row r="11" spans="1:7" ht="57.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>177</v>
+        <v>266</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="22" t="s">
-        <v>211</v>
+        <v>280</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>179</v>
+        <v>282</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -2105,14 +2236,14 @@
         <v>86</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>182</v>
@@ -2128,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95F4A8A-E29B-4E18-8E69-E97113C33CFB}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2145,7 +2276,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30">
       <c r="A1" s="27" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>4</v>
@@ -2171,17 +2302,17 @@
         <v>9</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G2" s="28"/>
     </row>
@@ -2190,36 +2321,36 @@
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="35" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="53.25">
+    <row r="4" spans="1:7" ht="100.5" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>190</v>
+        <v>265</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>242</v>
+        <v>288</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>243</v>
+        <v>289</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>154</v>
+        <v>290</v>
       </c>
       <c r="G4" s="13"/>
     </row>
@@ -2228,93 +2359,95 @@
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>264</v>
+        <v>291</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="24" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>266</v>
+        <v>293</v>
       </c>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:7" ht="178.5">
+    <row r="6" spans="1:7">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>235</v>
+        <v>294</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="D6" s="14"/>
+        <v>294</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>294</v>
+      </c>
       <c r="E6" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>200</v>
+        <v>294</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>294</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="25.5">
+    <row r="7" spans="1:7" ht="67.5">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>263</v>
+        <v>295</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>267</v>
+        <v>296</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>269</v>
+        <v>297</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="55.5" customHeight="1">
+    <row r="8" spans="1:7" ht="82.5" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>263</v>
+        <v>298</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="24" t="s">
-        <v>270</v>
+      <c r="E8" s="35" t="s">
+        <v>299</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>271</v>
+        <v>300</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="178.5">
+    <row r="9" spans="1:7" ht="27">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>168</v>
+        <v>265</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>242</v>
+        <v>288</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>243</v>
+        <v>301</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>252</v>
+        <v>302</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -2323,33 +2456,33 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="34" t="s">
-        <v>272</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>273</v>
+      <c r="E10" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>305</v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="51">
+    <row r="11" spans="1:7" ht="110.25" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>177</v>
+        <v>306</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="22" t="s">
-        <v>211</v>
+        <v>307</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>179</v>
@@ -2361,14 +2494,269 @@
         <v>86</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>263</v>
+        <v>308</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>274</v>
+        <v>309</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>268</v>
+        <v>310</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE04E62-3F20-49FE-92C9-574EE772D882}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.5">
+      <c r="A2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="1:7" ht="25.5">
+      <c r="A3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="35" t="s">
+        <v>313</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="100.5" customHeight="1">
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="130.5" customHeight="1">
+      <c r="A5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="63.75">
+      <c r="A7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="82.5" customHeight="1">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="25.5">
+      <c r="A9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="85.5" customHeight="1">
+      <c r="A10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="110.25" customHeight="1">
+      <c r="A11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="141" customHeight="1">
+      <c r="A12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>310</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>182</v>
@@ -3698,7 +4086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72FD7D6-2E49-4D32-923A-F7B61A1B2E55}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -3951,7 +4339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD081811-85A5-4B2D-B88E-0FFF35F2A58F}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -4158,19 +4546,15 @@
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>176</v>
-      </c>
+      <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>177</v>
+        <v>232</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>179</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="F11" s="12"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="87" customHeight="1">
@@ -4178,14 +4562,14 @@
         <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>182</v>
@@ -4201,8 +4585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8529FBE3-AC7C-4AEE-8C76-4DFCE0A834B0}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15"/>
@@ -4241,17 +4625,17 @@
         <v>9</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G2" s="28"/>
     </row>
@@ -4260,17 +4644,17 @@
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>218</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="13" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -4282,11 +4666,11 @@
         <v>190</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>154</v>
@@ -4300,15 +4684,13 @@
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="14" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>196</v>
-      </c>
+      <c r="E5" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="F5" s="13"/>
       <c r="G5" s="29"/>
       <c r="H5" s="13"/>
     </row>
@@ -4317,10 +4699,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14" t="s">
@@ -4337,14 +4719,14 @@
       </c>
       <c r="B7" s="31"/>
       <c r="C7" s="14" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -4354,13 +4736,15 @@
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="F8" s="13"/>
+        <v>253</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>154</v>
+      </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="191.25" customHeight="1">
@@ -4371,14 +4755,14 @@
         <v>168</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -4387,11 +4771,11 @@
         <v>23</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="22" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="4"/>
@@ -4400,19 +4784,15 @@
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>176</v>
-      </c>
+      <c r="B11" s="14"/>
       <c r="C11" s="14" t="s">
-        <v>177</v>
+        <v>252</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>179</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="F11" s="13"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="87" customHeight="1">
@@ -4420,14 +4800,14 @@
         <v>86</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Timesheet Update by Kavin
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet 1.xlsx
+++ b/Process/Timesheet/PTW-Timesheet 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74C05F2A-7036-4576-84F1-970A68AEFA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{240A5F70-9D98-426C-A63C-CEEE803F8AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="18-04-22" sheetId="51" r:id="rId10"/>
     <sheet name="19-04-22 " sheetId="52" r:id="rId11"/>
     <sheet name="20-04-22" sheetId="53" r:id="rId12"/>
-    <sheet name="21-04-22 " sheetId="54" r:id="rId13"/>
+    <sheet name="21-04-22" sheetId="54" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="381">
   <si>
     <t>Resource Name</t>
   </si>
@@ -937,6 +937,18 @@
     <t>Exploration on Angular, Entity Framework</t>
   </si>
   <si>
+    <t>HLD(services,components),typescript exploration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLD </t>
+  </si>
+  <si>
+    <t>meeting with team-30 mins(HLD),(services,components,data history)-1hr</t>
+  </si>
+  <si>
+    <t>Preparing for review-3hrs,self exploration-2 hrs.total-5 hrs</t>
+  </si>
+  <si>
     <t>angular exploration</t>
   </si>
   <si>
@@ -1034,22 +1046,62 @@
     <t xml:space="preserve">lunch and break 1hr 30mins, clearing others doubts - 2hrs </t>
   </si>
   <si>
-    <t>Layout for Head</t>
+    <t>Layout for TMS</t>
+  </si>
+  <si>
+    <t>Team Discussion about HLD - 30mins, Meeting with Rafi - 45mins, Session with Rafi about Services - 35mins, Team Discussion for split the works - 30mins, Bootstrap tutorial - 120mins</t>
+  </si>
+  <si>
+    <t>Softskills - 60mins, Lunch and Tea break - 90min,</t>
   </si>
   <si>
     <t>Interactions in HLD</t>
   </si>
   <si>
+    <t xml:space="preserve">               </t>
+  </si>
+  <si>
     <t xml:space="preserve">30mins : Team discussion, 45 mins : Meeting With Rafi, 35mins : Session about HLD and services, 30mins : Team discussion for splitting the topics and doubt clarification, 1 hr :System Architecture and NFA for HLD  </t>
   </si>
   <si>
     <t>3omis : Component concept in Angular,1 hrs : Softskill session,1.30 mins : Break time</t>
   </si>
   <si>
-    <t>Layout for Co-ordinator</t>
-  </si>
-  <si>
-    <t>Softskill session - 1 hr, Break  - 1:30 mins</t>
+    <t>Meeting with Rafi-45 Min,Team discussion for splitting the topics-60 min,Session About Services and HLD-30 min,Recall the previous day work-30 min,Bootstrap tutorial-120 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Softskill session - 1 hr, Break  - 1:15 hours </t>
+  </si>
+  <si>
+    <t>Created services for (Department,role)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team meeting - 30mins, Meeting with Rafi-45 mins,  Updated MOM,Worked on Services- 2 hours </t>
+  </si>
+  <si>
+    <t>Softskills session - 1 hours , Others (Lunch and break - 1 hour 30 mins)</t>
+  </si>
+  <si>
+    <t>exploration on web api,angular concepts</t>
+  </si>
+  <si>
+    <t>Databse Diagram for   TMS(user,course,topic,role,review,reviewstatus,department)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting with Rafi - 45 mins
+Team Discussion : 1 hr
+Worked on DB Diagram - 2.5 hr
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soft skill session - 1hr 
+Lunch and Teabreak-1.5hr</t>
+  </si>
+  <si>
+    <t>team discussion on HLD-30min, meeting with rafi-45min, session on services and HLD-30min,discussion with team to split work-30min, bootstrap tutorial- 140mis.</t>
+  </si>
+  <si>
+    <t>lunch -1.30hr ,  desgin pattern discussion with rafi(flyweight) -60min</t>
   </si>
   <si>
     <t>Services and dependencies in HLD</t>
@@ -1061,16 +1113,122 @@
     <t>Softskill session - 1 hr,  break - 1:30 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">Creating database ,tables,attributes and its description </t>
-  </si>
-  <si>
-    <t>Creating class files for services</t>
-  </si>
-  <si>
-    <t>Team meeting -30 min , Client meeting - 45 mins ,Class files for services - 2 hrs, Updating MOM - 15 mins</t>
+    <t>Created Database and Database Diagram for   TMS(Attendance,assignment,CourseFeedback,Mom,TraineeFeedback,Momstatus,attendancestatus,assignmentstatus,CoursetraineeMapping)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team discussion - 30min, Meeting with client -45 min, Worked in Database diagram-2.30min </t>
+  </si>
+  <si>
+    <t>Softskill session -1hr,Lunch -45mins,Break-20 min</t>
+  </si>
+  <si>
+    <t>Creating class files for services(User,Course,Review)</t>
+  </si>
+  <si>
+    <t>Team meeting -30 min , Client meeting - 35 mins ,Class files for services - 2 hrs, Updating MOM - 15 mins</t>
   </si>
   <si>
     <t>lunch and others 90mins, Angular component binding - 1 hr, WebApi - 1hr, softskill session - 1hr</t>
+  </si>
+  <si>
+    <t>web api(Department)</t>
+  </si>
+  <si>
+    <t>review the services,</t>
+  </si>
+  <si>
+    <t>meeting with team-20mins (spliting the teams),meeting with rafi-61 mins ,meeting with team work completion-20mins,working on web api(review)-2hrs,totla time spent-3hrs 41 mins</t>
+  </si>
+  <si>
+    <t>exploring on web api(2 hrs),break-40 mins,total -2hrs 40 mins</t>
+  </si>
+  <si>
+    <t>Layout for TMS except Head navbar</t>
+  </si>
+  <si>
+    <t>Layout for Head Navbar</t>
+  </si>
+  <si>
+    <t>Team Discussion about Work progress - 20mins, Meeting with Rafi - 60mins, Team Discussion for Work plan and team split - 30mins, Working and  Alteration on Head Layout 140mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunch and Tea break-75min  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">working on Web API </t>
+  </si>
+  <si>
+    <t>Refining System Architecture and Interaction for HLD</t>
+  </si>
+  <si>
+    <t>20 mins : Team discussion, 1hr : Meeting With Rafi,30mis : Team discussion and clarifying doubts,1.30 hr : Refining System Architecture and Interaction for HLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1hr : Exploring about Web API and connecting the DB, 1.30 mins : Lunch and Break </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layouts of TMS Co-ordinator </t>
+  </si>
+  <si>
+    <t>Layout for head nav bar</t>
+  </si>
+  <si>
+    <t>Team discussion-20 min,Meeting with Rafi-60 min,Discussion about Database diagram-30 min,Team discussion and Doubt-30 min</t>
+  </si>
+  <si>
+    <t>Lunch and Break-90 min,Boot strap about nav bar explortion-2 hours</t>
+  </si>
+  <si>
+    <t>Learning Web Api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed Services </t>
+  </si>
+  <si>
+    <t>Team discussion - 20 mins, Worked on Services(Department and role) - 2 hours, Meeting with Rafi - 1 hour, Doubt clarification meeting - 30 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watched Web api tutorial - 1 hour , Others(lunch and break) - 1 hour </t>
+  </si>
+  <si>
+    <t>Database diagram for TMS</t>
+  </si>
+  <si>
+    <t>Team Discussion-20mins
+Review Meeting with Rafi-1hr
+Refining the database diagram-10mins
+Understanding the services and methods in services-30mins
+Understanding the system architecture and interaction -30mins
+Team Discussion-30 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Lunch &amp; Tea break - 1.5 hr
+Exploration on Web API - 1 hr</t>
+  </si>
+  <si>
+    <t>layout for ( co-ordinator,trainer,trainee)</t>
+  </si>
+  <si>
+    <t>layout for training head</t>
+  </si>
+  <si>
+    <t>team disussion (progress) -20mim, meeting with rafi-60min, team discussion (team segeration)-30min, working on layout for training head-150min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lunch -1.15hrs </t>
+  </si>
+  <si>
+    <t>Working in layout for TMS</t>
+  </si>
+  <si>
+    <t>System architecture for HLD</t>
+  </si>
+  <si>
+    <t>Team discussion - 20 mins, meeting with rafi - 1hr,Team meeting and doubt clarification- 30 mins, worked with system architecture and interactions in HLD - 1:30 hr</t>
+  </si>
+  <si>
+    <t>Explored on bootstrap - 40 mins,break - 1 hr</t>
   </si>
   <si>
     <t>Building service for Department</t>
@@ -1089,7 +1247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1195,6 +1353,29 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1204,7 +1385,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1271,11 +1452,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1381,6 +1586,25 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2296,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95F4A8A-E29B-4E18-8E69-E97113C33CFB}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K4" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2339,17 +2563,17 @@
         <v>9</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>237</v>
+        <v>284</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>260</v>
+        <v>286</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="G2" s="28"/>
     </row>
@@ -2358,17 +2582,17 @@
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="35" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -2380,14 +2604,14 @@
         <v>265</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="G4" s="13"/>
     </row>
@@ -2399,14 +2623,14 @@
         <v>265</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="24" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G5" s="29"/>
     </row>
@@ -2415,19 +2639,19 @@
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -2436,17 +2660,17 @@
         <v>20</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
         <v>274</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -2455,17 +2679,17 @@
         <v>21</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>265</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -2477,14 +2701,14 @@
         <v>265</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -2496,14 +2720,14 @@
         <v>265</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="24" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -2515,11 +2739,11 @@
         <v>265</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="22" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>179</v>
@@ -2531,14 +2755,14 @@
         <v>86</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>182</v>
@@ -2552,24 +2776,24 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE04E62-3F20-49FE-92C9-574EE772D882}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" customWidth="1"/>
     <col min="6" max="6" width="30.85546875" customWidth="1"/>
     <col min="7" max="7" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -2592,233 +2816,221 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5">
+    <row r="2" spans="1:10" ht="18.75">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="G2" s="28"/>
-    </row>
-    <row r="3" spans="1:7" ht="25.5">
+      <c r="B2" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+    </row>
+    <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="35" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="100.5" customHeight="1">
+    <row r="4" spans="1:10" ht="100.5" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>289</v>
+        <v>320</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" ht="130.5" customHeight="1">
+    <row r="5" spans="1:10" ht="90" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>291</v>
+        <v>323</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="35" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="G5" s="29"/>
-    </row>
-    <row r="6" spans="1:7" ht="25.5">
+      <c r="J5" s="40"/>
+    </row>
+    <row r="6" spans="1:10" ht="56.25" customHeight="1">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="E6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="38" t="s">
+        <v>326</v>
+      </c>
       <c r="F6" s="14" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="61.5">
+    <row r="7" spans="1:10" ht="54.75" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>295</v>
-      </c>
+      <c r="B7" s="23"/>
       <c r="C7" s="33" t="s">
-        <v>296</v>
+        <v>328</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>274</v>
+        <v>329</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>297</v>
+        <v>330</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="82.5" customHeight="1">
+    <row r="8" spans="1:10" ht="110.25" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>265</v>
+        <v>331</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>332</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>299</v>
+        <v>333</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>300</v>
+        <v>334</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="25.5">
+    <row r="9" spans="1:10" ht="51">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>288</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>301</v>
+        <v>335</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>302</v>
+        <v>336</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="85.5" customHeight="1">
+    <row r="10" spans="1:10" ht="85.5" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="24" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="110.25" customHeight="1">
+    <row r="11" spans="1:10" ht="110.25" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="14" t="s">
-        <v>324</v>
+      <c r="C11" s="41" t="s">
+        <v>340</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="22" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>179</v>
+        <v>342</v>
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="141" customHeight="1">
+    <row r="12" spans="1:10" ht="141" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>326</v>
+        <v>344</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="G12" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C34C68-DFF4-4A4E-A0A5-F4D186552500}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE4816C-CAE5-4525-AB01-5036960B55BC}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
-    <col min="6" max="7" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="30">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -2841,202 +3053,214 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5">
+    <row r="2" spans="1:7" ht="63.75">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>237</v>
+        <v>346</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>259</v>
+        <v>347</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>260</v>
+        <v>348</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:7" ht="25.5">
+        <v>349</v>
+      </c>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="1:7" ht="53.25">
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>312</v>
+        <v>288</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>289</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="35" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:7" ht="100.5" customHeight="1">
+        <v>291</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="78.75" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="C4" s="14"/>
+        <v>350</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>351</v>
+      </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>289</v>
+        <v>352</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>290</v>
+        <v>353</v>
       </c>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" ht="130.5" customHeight="1">
+    <row r="5" spans="1:7" ht="71.25" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>316</v>
+        <v>354</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>291</v>
+        <v>355</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="35" t="s">
-        <v>317</v>
+        <v>356</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" ht="25.5">
+        <v>357</v>
+      </c>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7" ht="53.25">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>319</v>
+        <v>358</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="E6" s="14"/>
+        <v>359</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="13" t="s">
+        <v>360</v>
+      </c>
       <c r="F6" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7">
+        <v>361</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="51">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="23" t="s">
+        <v>362</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>363</v>
+      </c>
       <c r="D7" s="14"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-    </row>
-    <row r="8" spans="1:7" ht="82.5" customHeight="1">
+      <c r="E7" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="135" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>265</v>
+        <v>366</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>299</v>
+        <v>367</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" ht="25.5">
+        <v>368</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="66" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>265</v>
+        <v>369</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>288</v>
+        <v>370</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>301</v>
+        <v>371</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="85.5" customHeight="1">
+        <v>372</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="89.25">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>321</v>
+        <v>373</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>303</v>
+        <v>374</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="24" t="s">
-        <v>322</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" ht="110.25" customHeight="1">
+      <c r="E10" s="35" t="s">
+        <v>375</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="76.5">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="14"/>
+      <c r="B11" s="14" t="s">
+        <v>265</v>
+      </c>
       <c r="C11" s="14" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="22" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:7" ht="141" customHeight="1">
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="57.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>328</v>
+        <v>377</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>329</v>
+        <v>378</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>330</v>
+        <v>379</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="G12" s="14"/>
+        <v>380</v>
+      </c>
+      <c r="G12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>